<commit_message>
fix column in tool
</commit_message>
<xml_diff>
--- a/asset/tool/data/hocphi.xlsx
+++ b/asset/tool/data/hocphi.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F4FBBF-2384-451A-B190-3258F83D4769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2137FFEC-841A-4BFC-864C-5E9A2209AB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8009,8 +8009,8 @@
   <dimension ref="A1:S102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8277,7 +8277,6 @@
         <v>370</v>
       </c>
       <c r="M5" s="17">
-        <f>7500000/2</f>
         <v>3750000</v>
       </c>
       <c r="N5" s="17" t="s">

</xml_diff>